<commit_message>
Making various notations and changes to lab data for recalcitrant labs.
</commit_message>
<xml_diff>
--- a/27_ketoacidosis/27_ketoacidosis_data.xlsx
+++ b/27_ketoacidosis/27_ketoacidosis_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Ketoacidosis</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Also, strangely, the patienthas a negative concentration of bicarbonate in his blood, which seems pretty odd</t>
+  </si>
+  <si>
+    <t>at V-fib</t>
   </si>
 </sst>
 </file>
@@ -494,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -537,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
Adding percentage differences to Lab 27
</commit_message>
<xml_diff>
--- a/27_ketoacidosis/27_ketoacidosis_data.xlsx
+++ b/27_ketoacidosis/27_ketoacidosis_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Ketoacidosis</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>at V-fib</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,10 +185,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -201,9 +212,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -495,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -542,8 +557,20 @@
       <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -568,8 +595,23 @@
       <c r="J3" s="4">
         <v>4.42</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="30.75" thickBot="1">
+      <c r="M3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N12" si="0">ABS((B3-H3)/B3)</f>
+        <v>5.4200542005426126E-4</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" ref="O3:O12" si="1">ABS((C3-I3)/C3)</f>
+        <v>3.9215686274510463E-3</v>
+      </c>
+      <c r="P3" s="8">
+        <f t="shared" ref="P3:P12" si="2">ABS((D3-J3)/D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -594,8 +636,23 @@
       <c r="J4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="45.75" thickBot="1">
+      <c r="M4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="8">
+        <f>ABS((B4-H4)/B4)</f>
+        <v>0.1295454545454546</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.23333333333333339</v>
+      </c>
+      <c r="P4" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -620,8 +677,23 @@
       <c r="J5" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="30.75" thickBot="1">
+      <c r="M5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" ref="N5:N12" si="3">ABS((B5-H5)/B5)</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="P5" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0004643962848296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -646,8 +718,23 @@
       <c r="J6" s="4">
         <v>27.93</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30.75" thickBot="1">
+      <c r="M6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="3"/>
+        <v>6.2499999999999982</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" si="2"/>
+        <v>0.92964558301216649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -672,8 +759,22 @@
       <c r="J7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="60.75" thickBot="1">
+      <c r="M7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" si="1"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="60.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -698,8 +799,22 @@
       <c r="J8" s="4">
         <v>47.94</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="60.75" thickBot="1">
+      <c r="M8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="3"/>
+        <v>0.92727272727272725</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="1"/>
+        <v>5.9737417943107149E-2</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="60.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -724,8 +839,22 @@
       <c r="J9" s="4">
         <v>6.47</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="60.75" thickBot="1">
+      <c r="M9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="3"/>
+        <v>0.73636363636363611</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="1"/>
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -750,8 +879,21 @@
       <c r="J10" s="4">
         <v>39.64</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="45.75" thickBot="1">
+      <c r="M10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.15633333333333327</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -776,8 +918,22 @@
       <c r="J11" s="4">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="45.75" thickBot="1">
+      <c r="M11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" si="3"/>
+        <v>0.10714285714285723</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="1"/>
+        <v>0.26829268292682923</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -802,8 +958,22 @@
       <c r="J12" s="4">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="M12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="3"/>
+        <v>1.538461538461533E-2</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="1"/>
+        <v>0.28037383177570085</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -818,7 +988,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:16">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>

</xml_diff>

<commit_message>
Adding colorcodes to Lab 27
</commit_message>
<xml_diff>
--- a/27_ketoacidosis/27_ketoacidosis_data.xlsx
+++ b/27_ketoacidosis/27_ketoacidosis_data.xlsx
@@ -203,6 +203,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -212,15 +215,55 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -512,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,16 +641,16 @@
       <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="8">
-        <f t="shared" ref="N3:N12" si="0">ABS((B3-H3)/B3)</f>
+      <c r="N3" s="5">
+        <f t="shared" ref="N3" si="0">ABS((B3-H3)/B3)</f>
         <v>5.4200542005426126E-4</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="5">
         <f t="shared" ref="O3:O12" si="1">ABS((C3-I3)/C3)</f>
         <v>3.9215686274510463E-3</v>
       </c>
-      <c r="P3" s="8">
-        <f t="shared" ref="P3:P12" si="2">ABS((D3-J3)/D3)</f>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P6" si="2">ABS((D3-J3)/D3)</f>
         <v>0</v>
       </c>
     </row>
@@ -639,15 +682,15 @@
       <c r="M4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="5">
         <f>ABS((B4-H4)/B4)</f>
         <v>0.1295454545454546</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="5">
         <f t="shared" si="1"/>
         <v>0.23333333333333339</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -680,15 +723,15 @@
       <c r="M5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="5">
         <f t="shared" ref="N5:N12" si="3">ABS((B5-H5)/B5)</f>
         <v>0.29999999999999993</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="5">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="5">
         <f t="shared" si="2"/>
         <v>1.0004643962848296</v>
       </c>
@@ -721,15 +764,15 @@
       <c r="M6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="5">
         <f t="shared" si="3"/>
         <v>6.2499999999999982</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="5">
         <f t="shared" si="1"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="5">
         <f t="shared" si="2"/>
         <v>0.92964558301216649</v>
       </c>
@@ -762,15 +805,15 @@
       <c r="M7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="5">
         <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="5">
         <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -802,15 +845,15 @@
       <c r="M8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="5">
         <f t="shared" si="3"/>
         <v>0.92727272727272725</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="5">
         <f t="shared" si="1"/>
         <v>5.9737417943107149E-2</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -842,15 +885,15 @@
       <c r="M9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="5">
         <f t="shared" si="3"/>
         <v>0.73636363636363611</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="5">
         <f t="shared" si="1"/>
         <v>0.63958333333333328</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -882,14 +925,14 @@
       <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="5">
         <f t="shared" si="1"/>
         <v>0.15633333333333327</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -921,15 +964,15 @@
       <c r="M11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="5">
         <f t="shared" si="3"/>
         <v>0.10714285714285723</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="5">
         <f t="shared" si="1"/>
         <v>0.26829268292682923</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="P11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -961,88 +1004,88 @@
       <c r="M12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="5">
         <f t="shared" si="3"/>
         <v>1.538461538461533E-2</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="5">
         <f t="shared" si="1"/>
         <v>0.28037383177570085</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="P12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1050,6 +1093,15 @@
     <mergeCell ref="A17:K18"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
+  <conditionalFormatting sqref="N3:P12">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>